<commit_message>
Last change to model and add pdf
</commit_message>
<xml_diff>
--- a/platforms.xlsx
+++ b/platforms.xlsx
@@ -966,7 +966,6 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -974,12 +973,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -988,6 +981,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1404,8 +1406,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I11" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" topLeftCell="F9" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1675,64 +1677,64 @@
       <c r="A6" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="18" t="s">
         <v>75</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F6" s="12" t="s">
+      <c r="F6" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="G6" s="12" t="s">
+      <c r="G6" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="H6" s="12" t="s">
+      <c r="H6" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="I6" s="12" t="s">
+      <c r="I6" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="J6" s="15" t="s">
+      <c r="J6" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="K6" s="16" t="s">
+      <c r="K6" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="L6" s="16" t="s">
+      <c r="L6" s="20" t="s">
         <v>95</v>
       </c>
-      <c r="M6" s="15" t="s">
+      <c r="M6" s="20" t="s">
         <v>96</v>
       </c>
-      <c r="N6" s="15" t="s">
+      <c r="N6" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="O6" s="15" t="s">
+      <c r="O6" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="P6" s="15" t="s">
+      <c r="P6" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="Q6" s="15" t="s">
+      <c r="Q6" s="20" t="s">
         <v>100</v>
       </c>
-      <c r="R6" s="15" t="s">
+      <c r="R6" s="20" t="s">
         <v>101</v>
       </c>
-      <c r="S6" s="15" t="s">
+      <c r="S6" s="20" t="s">
         <v>102</v>
       </c>
-      <c r="T6" s="15" t="s">
+      <c r="T6" s="20" t="s">
         <v>103</v>
       </c>
-      <c r="U6" s="17" t="s">
+      <c r="U6" s="14" t="s">
         <v>104</v>
       </c>
       <c r="V6" s="2" t="s">
@@ -1746,10 +1748,10 @@
       <c r="A7" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="12" t="s">
         <v>78</v>
       </c>
       <c r="D7" s="2" t="s">
@@ -1761,27 +1763,27 @@
       <c r="F7" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G7" s="12"/>
+      <c r="G7" s="11"/>
     </row>
     <row r="8" spans="1:23" ht="195.75" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="D8" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="E8" s="14" t="s">
+      <c r="E8" s="13" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:23" ht="240" x14ac:dyDescent="0.25">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="13" t="s">
         <v>107</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -1801,7 +1803,7 @@
       </c>
     </row>
     <row r="10" spans="1:23" ht="195" x14ac:dyDescent="0.35">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="13" t="s">
         <v>115</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -1816,7 +1818,7 @@
       <c r="E10" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="F10" s="18" t="s">
+      <c r="F10" s="15" t="s">
         <v>120</v>
       </c>
       <c r="G10" s="2" t="s">
@@ -1831,7 +1833,7 @@
       <c r="J10" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="K10" s="19" t="s">
+      <c r="K10" s="16" t="s">
         <v>125</v>
       </c>
       <c r="L10" s="2" t="s">
@@ -1872,7 +1874,7 @@
       </c>
     </row>
     <row r="11" spans="1:23" ht="240" x14ac:dyDescent="0.35">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="13" t="s">
         <v>137</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -1905,7 +1907,7 @@
       <c r="K11" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="L11" s="20"/>
+      <c r="L11" s="17"/>
     </row>
     <row r="12" spans="1:23" ht="180" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">

</xml_diff>